<commit_message>
updated main.py to collapse args and updated evals
</commit_message>
<xml_diff>
--- a/results/test1/raw_outputs/claude-opus_outputs.xlsx
+++ b/results/test1/raw_outputs/claude-opus_outputs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE26"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,72 +521,47 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>class_period_score</t>
+          <t>causes_f1</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>causes_f1</t>
+          <t>composite_f1</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>composite_f1</t>
+          <t>prompt_tokens</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>prompt_tokens</t>
+          <t>completion_tokens</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>completion_tokens</t>
+          <t>cause_7</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>cause_7</t>
+          <t>cause_8</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>cause_8</t>
+          <t>cause_9</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>cause_9</t>
+          <t>cause_10</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>cause_10</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
           <t>cause_11</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>cause_12</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>cause_13</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>cause_14</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>cause_15</t>
         </is>
       </c>
     </row>
@@ -631,32 +606,32 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and Rule 10b-5</t>
+          <t>Violations of Section 10(b) of the Exchange Act and Rule 10b-5</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Exchange Act</t>
+          <t>Violations of Section 20(a) of the Exchange Act</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Section 20(A) of the Exchange Act</t>
+          <t>Violations of Section 20(A) of the Exchange Act</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Section 11 of the Securities Act</t>
+          <t>Violations of Section 11 of the Securities Act</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Section 12(a)(2) of the Securities Act</t>
+          <t>Violations of Section 12(a)(2) of the Securities Act</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Section 15 of the Securities Act</t>
+          <t>Violations of Section 15 of the Securities Act</t>
         </is>
       </c>
       <c r="O2" t="n">
@@ -669,29 +644,22 @@
         <v>1</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>0.889</v>
       </c>
       <c r="S2" t="n">
-        <v>0.889</v>
+        <v>0.789</v>
       </c>
       <c r="T2" t="n">
-        <v>0.789</v>
+        <v>112704</v>
       </c>
       <c r="U2" t="n">
-        <v>112842</v>
-      </c>
-      <c r="V2" t="n">
-        <v>231</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -734,12 +702,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Securities Exchange Act of 1934 and SEC Rule 10b-5</t>
+          <t>Violation of Section 10(b) of the Securities Exchange Act of 1934 and SEC Rule 10b-5 (against Tesla and Musk)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Securities Exchange Act of 1934</t>
+          <t>Violation of Section 20(a) of the Securities Exchange Act of 1934 (against the Board of Directors)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
@@ -756,29 +724,22 @@
         <v>1</v>
       </c>
       <c r="R3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
+        <v>0.667</v>
       </c>
       <c r="T3" t="n">
-        <v>0.667</v>
+        <v>29718</v>
       </c>
       <c r="U3" t="n">
-        <v>29856</v>
-      </c>
-      <c r="V3" t="n">
-        <v>195</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -821,12 +782,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5</t>
+          <t>Violation of Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5 promulgated thereunder</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Securities Exchange Act of 1934</t>
+          <t>Violation of Section 20(a) of the Securities Exchange Act of 1934</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -843,34 +804,27 @@
         <v>1</v>
       </c>
       <c r="R4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>0</v>
+        <v>0.582</v>
       </c>
       <c r="T4" t="n">
-        <v>0.582</v>
+        <v>47650</v>
       </c>
       <c r="U4" t="n">
-        <v>47788</v>
-      </c>
-      <c r="V4" t="n">
-        <v>149</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="inlineStr"/>
-      <c r="AD4" t="inlineStr"/>
-      <c r="AE4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>cand_22_cv_00105</t>
+          <t>cand_22_cv_02094</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -883,89 +837,74 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Martin Dugan; Leon Yu; Max Wisdom Technology Limited</t>
+          <t>Sjunde AP-Fonden (AP7)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Talis Biomedical Corporation; Brian Coe; J. Roger Moody, Jr.; Felix Baker; Raymond Cheong; Melissa Gilliam; Rustem F. Ismagilov; Kimberly J. Popovits; Matthew L. Posard; Randal Scott; Robert J. Kelley</t>
+          <t>Lucid Group, Inc.; Peter Rawlinson; Sherry House</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>TLIS</t>
+          <t>LCID</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2021-03-30</t>
+          <t>2021-11-15</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2022-03-15</t>
+          <t>2022-08-03</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Section 11 of the Securities Act of 1933</t>
+          <t>Violation of Section 10(b) of the Exchange Act and SEC Rule 10b-5</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Section 15 of the Securities Act of 1933</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Section 20(a) of the Securities Exchange Act of 1934</t>
-        </is>
-      </c>
+          <t>Violation of Section 20(a) of the Exchange Act</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
         <v>1</v>
       </c>
       <c r="P5" t="n">
-        <v>0.8179999999999999</v>
+        <v>0.857</v>
       </c>
       <c r="Q5" t="n">
         <v>1</v>
       </c>
       <c r="R5" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>0.871</v>
       </c>
       <c r="T5" t="n">
-        <v>0.764</v>
+        <v>83964</v>
       </c>
       <c r="U5" t="n">
-        <v>43871</v>
-      </c>
-      <c r="V5" t="n">
-        <v>254</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
-      <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="inlineStr"/>
-      <c r="AE5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>cand_22_cv_02094</t>
+          <t>cand_23_cv_02560</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -978,37 +917,37 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sjunde AP-Fonden</t>
+          <t>New England Teamsters Pension Fund</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Lucid Group, Inc.; Peter Rawlinson; Sherry House</t>
+          <t>Cutera, Inc.; David Mowry; Rohan Seth; J. Daniel Plants; Sheila Hopkins; Taylor Harris; Stuart Drummond; Vikram Varma</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>LCID</t>
+          <t>CUTR</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2021-11-15</t>
+          <t>2022-03-01</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2022-08-03</t>
+          <t>2024-03-21</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and SEC Rule 10b-5</t>
+          <t>Violation of Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5(b) promulgated thereunder</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Exchange Act</t>
+          <t>Violation of Section 20(a) of the Securities Exchange Act of 1934</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
@@ -1019,40 +958,33 @@
         <v>1</v>
       </c>
       <c r="P6" t="n">
-        <v>0.857</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="Q6" t="n">
         <v>1</v>
       </c>
       <c r="R6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>0.5</v>
+        <v>0.788</v>
       </c>
       <c r="T6" t="n">
-        <v>0.871</v>
+        <v>73598</v>
       </c>
       <c r="U6" t="n">
-        <v>84102</v>
-      </c>
-      <c r="V6" t="n">
-        <v>117</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="inlineStr"/>
-      <c r="AE6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>cand_23_cv_02560</t>
+          <t>cand_23_cv_03518</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1065,81 +997,82 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>New England Teamsters Pension Fund</t>
+          <t>Dr. Myo Thant; Branden Schenkhuizen</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Cutera, Inc.; David Mowry; Rohan Seth; J. Daniel Plants; Sheila Hopkins; Taylor Harris; Stuart Drummond; Vikram Varma</t>
+          <t>Rain Oncology Inc. f/k/a Rain Therapeutics Inc.; Avanish Vellanki; Richard Bryce; Franklin Berger; Aaron Davis; Gorjan Hrustanovic; Tran Nguyen; Peter Radovich; Stefani A. Wolff</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CUTR</t>
+          <t>RAIN</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2022-03-01</t>
+          <t>2021-04-23</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2024-03-21</t>
+          <t>2023-05-19</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and Rule 10b-5</t>
+          <t>Violation of Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5 promulgated thereunder</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Exchange Act</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+          <t>Violation of Section 20(a) of the Securities Exchange Act of 1934</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Violation of Section 11 of the Securities Act of 1933</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Violation of Section 15 of the Securities Act of 1933</t>
+        </is>
+      </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
         <v>1</v>
       </c>
       <c r="P7" t="n">
-        <v>0.9409999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="n">
         <v>1</v>
       </c>
       <c r="R7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="T7" t="n">
-        <v>0.988</v>
+        <v>35198</v>
       </c>
       <c r="U7" t="n">
-        <v>73736</v>
-      </c>
-      <c r="V7" t="n">
-        <v>169</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="inlineStr"/>
-      <c r="AD7" t="inlineStr"/>
-      <c r="AE7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>cand_23_cv_03518</t>
+          <t>cand_24_cv_03170</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1152,89 +1085,74 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Dr. Myo Thant; Branden Schenkhuizen</t>
+          <t>Lead Plaintiff; Ken Kula</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Rain Oncology Inc.; Rain Therapeutics Inc.; Avanish Vellanki; Richard Bryce; Franklin Berger; Aaron Davis; Gorjan Hrustanovic; Tran Nguyen; Peter Radovich; Stefani A. Wolff</t>
+          <t>Fastly, Inc.; Todd Nightingale; Ronald Kisling</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>RAIN</t>
+          <t>FSLY</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2021-04-23</t>
+          <t>2023-11-15</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2023-05-19</t>
+          <t>2024-08-07</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Section 10(b) and Rule 10b-5 of the Securities Exchange Act of 1934</t>
+          <t>Violations of Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5 promulgated thereunder</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Securities Exchange Act of 1934</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Section 11 of the Securities Act of 1933</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Section 15 of the Securities Act of 1933</t>
-        </is>
-      </c>
+          <t>Violations of Section 20(a) of the Securities Exchange Act of 1934</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P8" t="n">
-        <v>0.842</v>
+        <v>0.857</v>
       </c>
       <c r="Q8" t="n">
         <v>1</v>
       </c>
       <c r="R8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>0</v>
+        <v>0.671</v>
       </c>
       <c r="T8" t="n">
-        <v>0.768</v>
+        <v>27016</v>
       </c>
       <c r="U8" t="n">
-        <v>35336</v>
-      </c>
-      <c r="V8" t="n">
-        <v>241</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="inlineStr"/>
-      <c r="AE8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>cand_24_cv_03170</t>
+          <t>cand_24_cv_04196</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1247,37 +1165,37 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Lead Plaintiff; Ken Kula</t>
+          <t>Daniel Pogrebinsky; Benjamin Pouladian; David Mead; Aaron Goldman; Dr. Vijaykumar Agrawal; Kent Maguire; Timothy McKillican; Zi Xu</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Fastly, Inc.; Todd Nightingale; Ronald Kisling</t>
+          <t>Vicor Corporation; Patrizio Vinciarelli</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>FSLY</t>
+          <t>VICR</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2023-11-15</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2024-08-07</t>
+          <t>2023-10-24</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5</t>
+          <t>Violations of Section 10(b) of the Exchange Act and Rule 10b-5(b)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Securities Exchange Act of 1934</t>
+          <t>Violations of Section 20 of the Exchange Act (Control Person Liability)</t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -1285,10 +1203,10 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P9" t="n">
-        <v>0.857</v>
+        <v>1</v>
       </c>
       <c r="Q9" t="n">
         <v>1</v>
@@ -1297,31 +1215,24 @@
         <v>1</v>
       </c>
       <c r="S9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9" t="n">
-        <v>0.671</v>
+        <v>12572</v>
       </c>
       <c r="U9" t="n">
-        <v>27154</v>
-      </c>
-      <c r="V9" t="n">
-        <v>151</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>cand_24_cv_04196</t>
+          <t>cand_3_22-cv-00956</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1334,37 +1245,37 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Daniel Pogrebinsky; Benjamin Pouladian; David Mead; Aaron Goldman; Dr. Vijaykumar Agrawal; Kent Maguire; Timothy McKillican; Zi Xu</t>
+          <t>Steamfitters Local 449 Pension &amp; Retirement Security Funds</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Vicor Corporation; Patrizio Vinciarelli</t>
+          <t>SunPower Corporation; Peter Faricy; Manavendra S. Sial</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>VICR</t>
+          <t>SPWR</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2023-07-25</t>
+          <t>2021-08-03</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2023-10-24</t>
+          <t>2022-01-20</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and Rule 10b-5(b)</t>
+          <t>Violation of Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5 promulgated thereunder</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Exchange Act</t>
+          <t>Violation of Section 20(a) of the Securities Exchange Act of 1934</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
@@ -1372,7 +1283,7 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
         <v>1</v>
@@ -1381,34 +1292,27 @@
         <v>1</v>
       </c>
       <c r="R10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="T10" t="n">
-        <v>1</v>
+        <v>22417</v>
       </c>
       <c r="U10" t="n">
-        <v>12710</v>
-      </c>
-      <c r="V10" t="n">
-        <v>220</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="inlineStr"/>
-      <c r="AE10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>cand_3_21-cv-09767</t>
+          <t>casd_3_23-cv-01216</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1421,44 +1325,40 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Vinod Sodha; Amee Sodha</t>
+          <t>Dipak Patel</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Robinhood Markets, Inc.; Vladimir Tenev; Jason Warnick; Baiju Bhatt; Jan Hammer; Paula Loop; Jonathan Rubenstein; Scott Sandell; Robert Zoellick; Goldman Sachs &amp; Co. LLC; J.P. Morgan Securities LLC; Barclays Capital Inc.; Citigroup Global Markets Inc.; Wells Fargo Securities, LLC; Mizuho Securities USA LLC; JMP Securities LLC; KeyBanc Capital Markets Inc.; Piper Sandler &amp; Co.; Rosenblatt Securities Inc.; BMO Capital Markets Corp.; BTIG, LLC; Santander Investment Securities Inc.; Academy Securities, Inc.; Loop Capital Markets LLC; Samuel A. Ramirez &amp; Company, Inc.; Siebert Williams Shank &amp; Co., LLC</t>
+          <t>ImmunityBio, Inc.; Richard Adcock; David C. Sachs; Patrick Soon-Shiong</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>HOOD</t>
+          <t>IBRX</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2021-07-28</t>
+          <t>2021-03-10</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2021-07-30</t>
+          <t>2023-05-10</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Section 11 of the Securities Act of 1933</t>
+          <t>Violations of Section 10(b) of the Securities Exchange Act of 1934 and SEC Rule 10b-5</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Section 12(a)(2) of the Securities Act of 1933</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Section 15 of the Securities Act of 1933</t>
-        </is>
-      </c>
+          <t>Violations of Section 20(a) of the Securities Exchange Act of 1934</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
@@ -1466,7 +1366,7 @@
         <v>1</v>
       </c>
       <c r="P11" t="n">
-        <v>0.923</v>
+        <v>0.889</v>
       </c>
       <c r="Q11" t="n">
         <v>1</v>
@@ -1475,31 +1375,24 @@
         <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>0</v>
+        <v>0.778</v>
       </c>
       <c r="T11" t="n">
-        <v>0.585</v>
+        <v>37432</v>
       </c>
       <c r="U11" t="n">
-        <v>33312</v>
-      </c>
-      <c r="V11" t="n">
-        <v>322</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr"/>
-      <c r="AB11" t="inlineStr"/>
-      <c r="AC11" t="inlineStr"/>
-      <c r="AD11" t="inlineStr"/>
-      <c r="AE11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>cand_3_22-cv-00956</t>
+          <t>ctd-3-23-cv-01035</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1512,37 +1405,37 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Steamfitters Local 449 Pension &amp; Retirement Security Funds</t>
+          <t>New England Teamsters Pension Fund; Westchester Putnam Counties Heavy &amp; Highway Laborers Local 60 Benefits Fund; United Union of Roofers, Waterproofers &amp; Allied Workers Local Union No. 8 WBPA Fund</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>SunPower Corporation; Peter Faricy; Manavendra S. Sial</t>
+          <t>RTX Corporation; Gregory Hayes; Neil Mitchill; Anthony F. O'Brien; Christopher T. Calio; Shane Eddy</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>SPWR</t>
+          <t>RTX</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2021-08-03</t>
+          <t>2021-02-08</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2022-01-20</t>
+          <t>2023-09-08</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and Rule 10b-5</t>
+          <t>Violations of Section 10(b) of the Securities Exchange Act of 1934 and SEC Rule 10b-5</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Exchange Act</t>
+          <t>Violations of Section 20(a) of the Securities Exchange Act of 1934</t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -1550,43 +1443,36 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
+        <v>0.286</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>1</v>
+      </c>
+      <c r="R12" t="n">
         <v>0</v>
       </c>
-      <c r="P12" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>1</v>
-      </c>
-      <c r="R12" t="n">
-        <v>1</v>
-      </c>
       <c r="S12" t="n">
-        <v>1</v>
+        <v>0.624</v>
       </c>
       <c r="T12" t="n">
-        <v>0.8</v>
+        <v>70186</v>
       </c>
       <c r="U12" t="n">
-        <v>22555</v>
-      </c>
-      <c r="V12" t="n">
-        <v>151</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
-      <c r="AC12" t="inlineStr"/>
-      <c r="AD12" t="inlineStr"/>
-      <c r="AE12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>casd_3_23-cv-01216</t>
+          <t>dcd-1_23-cv-02055</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1599,37 +1485,37 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Dipak Patel</t>
+          <t>Derek Einersen</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ImmunityBio, Inc.; Richard Adcock; David C. Sachs; Patrick Soon-Shiong</t>
+          <t>Danaher Corporation; Rainer M. Blair; Matthew R. McGrew; Emmanuel Ligner</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>IBRX</t>
+          <t>DHR</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2021-03-10</t>
+          <t>2022-01-27</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2023-05-10</t>
+          <t>2023-10-23</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Securities Exchange Act of 1934 and SEC Rule 10b-5</t>
+          <t>Violations of Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5 promulgated thereunder</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Securities Exchange Act of 1934</t>
+          <t>Violations of Section 20(a) of the Securities Exchange Act of 1934</t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -1637,43 +1523,36 @@
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>0.889</v>
+        <v>0.75</v>
       </c>
       <c r="Q13" t="n">
         <v>1</v>
       </c>
       <c r="R13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="T13" t="n">
-        <v>0.778</v>
+        <v>39827</v>
       </c>
       <c r="U13" t="n">
-        <v>37570</v>
-      </c>
-      <c r="V13" t="n">
-        <v>162</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="V13" t="inlineStr"/>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ctd-3_24-cv-01727</t>
+          <t>dde_ 23_cv_1466</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1686,125 +1565,78 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Securities and Exchange Commission</t>
+          <t>AltShares Event-Driven ETF; AltShares Merger Arbitrage ETF; Kryger Event Fund Ltd.; Kryger Enhanced Fund Ltd.; ODS Capital LLC</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Lovesac; Donna Dellomo; Yoon Um</t>
+          <t>Focus Financial Partners Inc.; George S. LeMieux; Elizabeth R. Neuhoff; Greg S. Morganroth, M.D.; Joseph Feliciani, Jr.; Ruediger 'Rudy' Adolf; Rajini Sundar Kodialam; James D. Carey; Fayez S. Muhtadie; James Shanahan; Leonard Chang; J. Russell McGranahan; Clayton, Dubilier &amp; Rice, LLC; Goldman Sachs &amp; Co. LLC; Jefferies LLC; Stone Point Capital LLC; Vinson &amp; Elkins L.L.P.; Potter Anderson &amp; Corroon LLP</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>LOVE</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+          <t>FOCS</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2023-08-31</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Securities Act Section 17(a)(1) - Fraud in the Offer or Sale of Securities</t>
+          <t>Violation of Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5(a)-(c) promulgated thereunder</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Securities Act Section 17(a)(3) - Fraud in the Offer or Sale of Securities</t>
+          <t>Violation of Section 14(a) of the Securities Exchange Act of 1934 and Rule 14a-9 promulgated thereunder</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Exchange Act Section 10(b) and Rules 10b-5(a) and (c) - Fraud in Connection with the Purchase or Sale of Securities</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Exchange Act Section 10(b) and Rule 10b-5(b) - Fraud in Connection with the Purchase or Sale of Securities</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>Aiding and Abetting violations of Exchange Act Section 10(b) and Rule 10b-5(b)</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>Exchange Act Section 13(b)(5) - Knowingly Circumventing Internal Controls, Failing to Implement Internal Controls, or Falsifying Books and Records</t>
-        </is>
-      </c>
+          <t>Violation of Section 20(a) of the Securities Exchange Act of 1934 (Control Person Liability)</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>1</v>
+      </c>
+      <c r="R14" t="n">
         <v>0</v>
       </c>
-      <c r="P14" t="n">
-        <v>0.667</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>1</v>
-      </c>
-      <c r="R14" t="n">
-        <v>1</v>
-      </c>
       <c r="S14" t="n">
-        <v>0.24</v>
+        <v>0.713</v>
       </c>
       <c r="T14" t="n">
-        <v>0.581</v>
+        <v>37752</v>
       </c>
       <c r="U14" t="n">
-        <v>13532</v>
-      </c>
-      <c r="V14" t="n">
-        <v>578</v>
-      </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>Exchange Act Rule 13b2-1 - Falsifying Any Book, Record, or Account</t>
-        </is>
-      </c>
-      <c r="X14" t="inlineStr">
-        <is>
-          <t>Exchange Act Rule 13b2-2 - Lying, Coercing, or Improperly Influencing an Accountant</t>
-        </is>
-      </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>Exchange Act Section 13(a) and Rules 12b-20, 13a-1, 13a-11, and 13a-13 - Material Misstatements or Omissions in Periodic or Other Reports</t>
-        </is>
-      </c>
-      <c r="Z14" t="inlineStr">
-        <is>
-          <t>Aiding and Abetting violations of Exchange Act Section 13(a) and Rules 12b-20, 13a-1, 13a-11, and 13a-13</t>
-        </is>
-      </c>
-      <c r="AA14" t="inlineStr">
-        <is>
-          <t>Exchange Act Rule 13a-14 - False Certification of Financial Reports</t>
-        </is>
-      </c>
-      <c r="AB14" t="inlineStr">
-        <is>
-          <t>Exchange Act Section 13(b)(2)(A) - Failure to Make and Keep Books and Records in Reasonable Detail</t>
-        </is>
-      </c>
-      <c r="AC14" t="inlineStr">
-        <is>
-          <t>Aiding and Abetting violations of Exchange Act Section 13(b)(2)(A)</t>
-        </is>
-      </c>
-      <c r="AD14" t="inlineStr">
-        <is>
-          <t>Exchange Act Section 13(b)(2)(B) - Failure to Devise and Maintain a System of Internal Accounting Controls</t>
-        </is>
-      </c>
-      <c r="AE14" t="inlineStr">
-        <is>
-          <t>Aiding and Abetting violations of Exchange Act Section 13(b)(2)(B)</t>
-        </is>
-      </c>
+        <v>457</v>
+      </c>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>dcd-1_23-cv-01599</t>
+          <t>dde_21_cv_55</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1817,113 +1649,74 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>U.S. Securities and Exchange Commission</t>
+          <t>Kim Kengle as trustee of the Kim K. Kengle 2000 Trust; Roseanne Lacy</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Binance Holdings Limited; BAM Trading Services Inc.; BAM Management US Holdings Inc.; Changpeng Zhao</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+          <t>Walmart Inc.; Douglas C. McMillon; M. Brett Biggs</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>WMT</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2017-03-31</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2020-12-22</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Sections 5(a) and 5(c) of the Securities Act - Unregistered Offers and Sales of BNB</t>
+          <t>Violations of Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5 promulgated thereunder</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Sections 5(a) and 5(c) of the Securities Act - Unregistered Offers and Sales of BUSD</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Sections 5(a) and 5(c) of the Securities Act - Unregistered Offer and Sale of Simple Earn and BNB Vault</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>Sections 5(a) and 5(c) of the Securities Act - Unregistered Offer and Sale of Staking Program</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>Exchange Act Section 5 - Failing to Register as an Exchange for the Binance.com Platform</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>Exchange Act Section 15(a) - Failing to Register as a Broker-Dealer for the Binance.com Platform</t>
-        </is>
-      </c>
+          <t>Violations of Section 20(a) of the Securities Exchange Act of 1934</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>1</v>
+        <v>0.857</v>
       </c>
       <c r="Q15" t="n">
         <v>1</v>
       </c>
       <c r="R15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>0</v>
+        <v>0.571</v>
       </c>
       <c r="T15" t="n">
-        <v>0.6</v>
+        <v>50878</v>
       </c>
       <c r="U15" t="n">
-        <v>58466</v>
-      </c>
-      <c r="V15" t="n">
-        <v>470</v>
-      </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>Exchange Act Section 17A(b) - Failing to Register as a Clearing Agency for the Binance.com Platform</t>
-        </is>
-      </c>
-      <c r="X15" t="inlineStr">
-        <is>
-          <t>Exchange Act Section 5 - Failure to Register as an Exchange for the Binance.US Platform</t>
-        </is>
-      </c>
-      <c r="Y15" t="inlineStr">
-        <is>
-          <t>Exchange Act Section 15(a) - Failing to Register as a Broker for the Binance.US Platform</t>
-        </is>
-      </c>
-      <c r="Z15" t="inlineStr">
-        <is>
-          <t>Exchange Act Section 17A(b) - Failing to Register as a Clearing Agency for the Binance.US Platform</t>
-        </is>
-      </c>
-      <c r="AA15" t="inlineStr">
-        <is>
-          <t>Exchange Act Sections 5, 15(a), and 17A(b) - Control Person Liability (Zhao for Binance.com Platform)</t>
-        </is>
-      </c>
-      <c r="AB15" t="inlineStr">
-        <is>
-          <t>Exchange Act Sections 5, 15(a), and 17A(b) - Control Person Liability (Zhao for Binance.US Platform)</t>
-        </is>
-      </c>
-      <c r="AC15" t="inlineStr">
-        <is>
-          <t>Securities Act Sections 17(a)(2) and (a)(3) - Fraud</t>
-        </is>
-      </c>
-      <c r="AD15" t="inlineStr"/>
-      <c r="AE15" t="inlineStr"/>
+        <v>209</v>
+      </c>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>dcd-1_23-cv-02055</t>
+          <t>flsd-1_23-cv-23139</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1936,81 +1729,98 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Derek Einersen</t>
+          <t>Kristoffer Jon Hind; Jason Thomas Waiton; Christopher Campbell; Paul Douglas Stoeppelwerth; Lucas Longmire; Thomas Blair Phillips; Tyler Jenkins; Jorden David Neil Malcolm; Robert Taylor Yates; Rafael Reyes Salmeron; Ryan Anthony Floyd; Matt Scott Vogel; Mark Alan Bentley; Peter Shane Donahue; Agata Agnieszka Powers; Avya Lindsey Waiton; Timothy Michael Morgan; Tarsis Carvalho Humphreys; Zachary Michael Sellers; Brandon Michael Harrold</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Danaher; Rainer M. Blair; Matthew R. McGrew; Emmanuel Ligner</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>DHR</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2022-01-27</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>2023-10-23</t>
-        </is>
-      </c>
+          <t>CFT Solutions, LLC; FxWinning Limited; Renan de Rocha Gomes Bastos; Rafael Brito Cutie; Arthur Percy; Roman Cardenas; David Merino</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5</t>
+          <t>Violation of the Securities Act of 1933, 15 U.S.C. § 77e and 77l(a)(1)</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Securities Exchange Act of 1934</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
+          <t>Violation of the Securities Exchange Act of 1934 and Rule 10b-5, 15 U.S.C. § 78j(b) and C.F.R. § 240.10b-5</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Violation of the Commodities Exchange Act, Sections 6 and 25, 7 U.S.C. §§ 6b, 6e, 6o, and 25</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Violation of the Florida Securities and Investor Protection Act, Sections 517.301 and 517.211</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Breach of Contract</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Breach of Fiduciary Duty</t>
+        </is>
+      </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" t="n">
-        <v>0.5</v>
+        <v>0.857</v>
       </c>
       <c r="Q16" t="n">
         <v>1</v>
       </c>
       <c r="R16" t="n">
-        <v>1</v>
+        <v>0.636</v>
       </c>
       <c r="S16" t="n">
-        <v>0</v>
+        <v>0.899</v>
       </c>
       <c r="T16" t="n">
-        <v>0.5</v>
+        <v>17996</v>
       </c>
       <c r="U16" t="n">
-        <v>39965</v>
-      </c>
-      <c r="V16" t="n">
-        <v>152</v>
-      </c>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="inlineStr"/>
-      <c r="AD16" t="inlineStr"/>
-      <c r="AE16" t="inlineStr"/>
+        <v>574</v>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>Fraud in the Inducement</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>Negligent Misrepresentations</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>Conversion</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>Unjust Enrichment</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>Civil Conspiracy</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>dde_ 23_cv_1466</t>
+          <t>ilnd-1-21-cv-04349</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2023,85 +1833,82 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>AltShares Event-Driven ETF; AltShares Merger Arbitrage ETF; Kryger Event Fund Ltd.; Kryger Enhanced Fund Ltd.; ODS Capital LLC</t>
+          <t>The Phoenix Insurance Company Ltd.; The Phoenix Pension &amp; Provident Funds; City of Melbourne Firefighters' Retirement System</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Focus Financial Partners Inc.; George S. LeMieux; Elizabeth R. Neuhoff; Greg S. Morganroth, M.D.; Joseph Feliciani, Jr.; Ruediger "Rudy" Adolf; Rajini Sundar Kodialam; James D. Carey; Fayez S. Muhtadie; James Shanahan; Leonard Chang; J. Russell McGranahan; Clayton, Dubilier &amp; Rice, LLC; Goldman Sachs &amp; Co. LLC; Jefferies LLC; Stone Point Capital LLC; Vinson &amp; Elkins L.L.P.; Potter Anderson &amp; Corroon LLP</t>
+          <t>ATI Physical Therapy, Inc. f/k/a Fortress Value Acquisition Corp. II; Labeed Diab; Joseph Jordan; Andrew A. McKnight; Joshua A. Pack; Marc Furstein; Leslee Cowen; Aaron F. Hood; Carmen A. Policy; Rakefet Russak-Aminoach; Sunil Gulati</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>FOCS</t>
+          <t>ATIP</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2023-02-27</t>
+          <t>2021-02-22</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2023-08-31</t>
+          <t>2021-10-19</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and Rule 10b-5(a)-(c)</t>
+          <t>Violations of Section 10(b) of the Securities Exchange Act of 1934 and SEC Rule 10b-5</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Section 14(a) of the Exchange Act and Rule 14a-9</t>
+          <t>Violations of Section 20(a) of the Securities Exchange Act of 1934 (Control Person Liability for Section 10(b) claims)</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Exchange Act</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr"/>
+          <t>Violations of Section 14(a) of the Securities Exchange Act of 1934 and SEC Rule 14a-9</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Violations of Section 20(a) of the Securities Exchange Act of 1934 (Control Person Liability for Section 14(a) claims)</t>
+        </is>
+      </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>1</v>
+        <v>0.667</v>
       </c>
       <c r="P17" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.87</v>
       </c>
       <c r="Q17" t="n">
         <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>0.8</v>
+        <v>0.707</v>
       </c>
       <c r="T17" t="n">
-        <v>0.872</v>
+        <v>34460</v>
       </c>
       <c r="U17" t="n">
-        <v>37890</v>
-      </c>
-      <c r="V17" t="n">
-        <v>412</v>
-      </c>
+        <v>379</v>
+      </c>
+      <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="inlineStr"/>
-      <c r="AB17" t="inlineStr"/>
-      <c r="AC17" t="inlineStr"/>
-      <c r="AD17" t="inlineStr"/>
-      <c r="AE17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>dde_21_cv_55</t>
+          <t>mad-1-21-cv-10933</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2114,37 +1921,37 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Kim Kengle as trustee of the Kim K. Kengle 2000 Trust; Roseanne Lacy</t>
+          <t>Julian Quinones</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Walmart Inc.; Douglas C. McMillon; M. Brett Biggs</t>
+          <t>Frequency Therapeutics, Inc.; David L. Lucchino; Carl LeBel</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>WMT</t>
+          <t>FREQ</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2017-03-31</t>
+          <t>2020-10-29</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2020-12-22</t>
+          <t>2021-03-23</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and Rule 10b-5</t>
+          <t>Violations of Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5 promulgated thereunder</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Exchange Act</t>
+          <t>Violations of Section 20(a) of the Securities Exchange Act of 1934 (against Individual Defendants)</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
@@ -2152,7 +1959,7 @@
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" t="n">
         <v>0.857</v>
@@ -2161,34 +1968,27 @@
         <v>1</v>
       </c>
       <c r="R18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>1</v>
+        <v>0.751</v>
       </c>
       <c r="T18" t="n">
-        <v>0.771</v>
+        <v>18128</v>
       </c>
       <c r="U18" t="n">
-        <v>51016</v>
-      </c>
-      <c r="V18" t="n">
-        <v>160</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="V18" t="inlineStr"/>
       <c r="W18" t="inlineStr"/>
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr"/>
-      <c r="AA18" t="inlineStr"/>
-      <c r="AB18" t="inlineStr"/>
-      <c r="AC18" t="inlineStr"/>
-      <c r="AD18" t="inlineStr"/>
-      <c r="AE18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>flsd-1_23-cv-23139</t>
+          <t>mied-4-23-cv-13132</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2201,105 +2001,82 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Kristoffer Jon Hind; Jason Thomas Waiton; Christopher Campbell; Paul Douglas Stoeppelwerth; Lucas Longmire; Thomas Blair Phillips; Tyler Jenkins; Jorden David Neil Malcolm; Robert Taylor Yates; Rafael Reyes Salmeron; Ryan Anthony Floyd; Matt Scott Vogel; Mark Alan Bentley; Peter Shane Donahue; Agata Agnieszka Powers; Avya Lindsey Waiton; Timothy Michael Morgan; Tarsis Carvalho Humphreys; Zachary Michael Sellers; Brandon Michael Harrold</t>
+          <t>City of Hollywood Police Officers' Retirement System; Plymouth County Retirement Association</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>CFT Solutions, LLC; FxWinning Limited; Renan de Rocha Gomes Bastos; Rafael Brito Cutie; Arthur Percy; Roman Cardenas; David Merino</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+          <t>General Motors Company; Cruise LLC; Mary T. Barra; Paul A. Jacobson; Kyle Vogt; Daniel Ammann; Doug L. Parks; Wayne G. West</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2021-02-24</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2023-11-08</t>
+        </is>
+      </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Violation of the Securities Act of 1933, 15 U.S.C. § 77e and 77l(a)(1)</t>
+          <t>Violations of Section 10(b) of the Exchange Act and Rule 10b-5(b)</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Violation of the Securities Exchange Act of 1934 and Rule 10b-5, 15 U.S.C. § 78j(b) and C.F.R. § 240.10b-5</t>
+          <t>Violations of Section 10(b) of the Exchange Act and Rule 10b-5(a)/(c)</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Violation of the Commodities Exchange Act, Sections 6 and 25, 7 U.S.C. §§ 6b, 6e, 6o, and 25</t>
+          <t>Violations of Section 20(a) of the Exchange Act against Defendants Barra, Jacobson, and Parks as Control Persons of GM</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Violation of the Florida Securities and Investor Protection Act, Sections 517.301 and 517.211</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Breach of Contract</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>Breach of Fiduciary Duty</t>
-        </is>
-      </c>
+          <t>Violations of Section 20(a) of the Exchange Act against the Individual Defendants as Control Persons of Cruise</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P19" t="n">
-        <v>0.857</v>
+        <v>1</v>
       </c>
       <c r="Q19" t="n">
         <v>1</v>
       </c>
       <c r="R19" t="n">
-        <v>1</v>
+        <v>0.571</v>
       </c>
       <c r="S19" t="n">
-        <v>0.636</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="T19" t="n">
-        <v>0.899</v>
+        <v>72073</v>
       </c>
       <c r="U19" t="n">
-        <v>18134</v>
-      </c>
-      <c r="V19" t="n">
-        <v>574</v>
-      </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>Fraud in the Inducement</t>
-        </is>
-      </c>
-      <c r="X19" t="inlineStr">
-        <is>
-          <t>Negligent Misrepresentations</t>
-        </is>
-      </c>
-      <c r="Y19" t="inlineStr">
-        <is>
-          <t>Conversion</t>
-        </is>
-      </c>
-      <c r="Z19" t="inlineStr">
-        <is>
-          <t>Unjust Enrichment</t>
-        </is>
-      </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>Civil Conspiracy</t>
-        </is>
-      </c>
-      <c r="AB19" t="inlineStr"/>
-      <c r="AC19" t="inlineStr"/>
-      <c r="AD19" t="inlineStr"/>
-      <c r="AE19" t="inlineStr"/>
+        <v>296</v>
+      </c>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ilnd-1_20_cv_05593</t>
+          <t>nysd_20_cv_04494</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2312,37 +2089,37 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Sudhakara R. Murikinati; Jerry Nixon; Benjamin Sandmann; Jeff S. Turnipseed</t>
+          <t>Handelsbanken Fonder AB; Public Employees' Retirement System of Mississippi; State of Rhode Island, Office of the General Treasurer, on behalf of the Employees' Retirement System of Rhode Island; Louisiana Sheriffs' Pension &amp; Relief Fund</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>GoHealth, Inc.; Clinton P. Jones; Brandon M. Cruz; Travis J. Matthiesen; NVX Holdings, Inc.; Centerbridge Partners, L.P.; CCP III AIV VII Holdings, L.P.; CB Blizzard Co-Invest Holdings, L.P.; Blizzard Aggregator, LLC; Centerbridge Associates III, L.P.; CCP III Cayman GP Ltd.; Goldman Sachs &amp; Co. LLC; BofA Securities, Inc.; Morgan Stanley &amp; Co. LLC</t>
+          <t>Wells Fargo &amp; Company; Timothy J. Sloan; John R. Shrewsberry; Charles W. Scharf; C. Allen Parker; Elizabeth Duke</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>GOCO</t>
+          <t>WFC</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2020-07-14</t>
+          <t>2018-02-02</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2020-07-17</t>
+          <t>2020-03-12</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Section 11 of the Securities Act of 1933</t>
+          <t>Violations of Section 10(b) of the Securities Exchange Act and SEC Rule 10b-5</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Section 15 of the Securities Act of 1933</t>
+          <t>Violations of Section 20(a) of the Securities Exchange Act</t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
@@ -2350,10 +2127,10 @@
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="P20" t="n">
-        <v>0.645</v>
+        <v>0.833</v>
       </c>
       <c r="Q20" t="n">
         <v>1</v>
@@ -2362,31 +2139,24 @@
         <v>0</v>
       </c>
       <c r="S20" t="n">
-        <v>0</v>
+        <v>0.607</v>
       </c>
       <c r="T20" t="n">
-        <v>0.529</v>
+        <v>57540</v>
       </c>
       <c r="U20" t="n">
-        <v>27761</v>
-      </c>
-      <c r="V20" t="n">
-        <v>271</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="V20" t="inlineStr"/>
       <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr"/>
-      <c r="AA20" t="inlineStr"/>
-      <c r="AB20" t="inlineStr"/>
-      <c r="AC20" t="inlineStr"/>
-      <c r="AD20" t="inlineStr"/>
-      <c r="AE20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>nysd_1_21-cv-11222</t>
+          <t>nysd_22-cv-07111</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2399,89 +2169,82 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>DarkPulse, Inc.</t>
+          <t>RTD Bros LLC; Todd Benn; Tom Benn; Tomasz Rzedzian; Preston Million</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>FirstFire Global Opportunity Fund, LLC; Eli Fireman; FirstFire Capital Management, LLC</t>
+          <t>Lottery.com, Inc.; Trident Acquisitions Corp.; Lawrence Anthony DiMatteo III; Ryan Dickinson; Matthew Clemenson; Kathryn Lever; Marat Rosenberg; Vadim Komissarov; Thomas Gallagher; Gennadii Butkevych; Ilya Ponomarev</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>DPLS</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+          <t>LTRY</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2020-11-19</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2022-07-29</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Section 29(b) of the Securities Exchange Act for Violating Section 15(a) by Effecting (Making) Transactions As an Unregistered Dealer</t>
+          <t>Violations of Section 10(b) of the Exchange Act and Rule 10b-5 Promulgated Thereunder</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Section 29(b) of the Securities Exchange Act for Violating Section 15(a) by Unlawfully Transacting in Securities Via Performance of the Agreements as an Unregistered Dealer</t>
+          <t>Violations of Section 20(a) of the Exchange Act</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Securities Exchange Act - Control Person Liability</t>
+          <t>Violation of Section 14(a) of the Exchange Act and Rule 14a-9</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>RICO Section 1962(c) - Conducting Affairs of the RICO Enterprise Through Collection of Unlawful Debt</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>Unjust Enrichment</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>Constructive Trust</t>
-        </is>
-      </c>
+          <t>Violation of Section 20(a) of the Exchange Act (related to Section 14(a) claims)</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>0.667</v>
+        <v>0.889</v>
       </c>
       <c r="P21" t="n">
-        <v>0</v>
+        <v>0.471</v>
       </c>
       <c r="Q21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21" t="n">
-        <v>1</v>
+        <v>0.571</v>
       </c>
       <c r="S21" t="n">
-        <v>0.333</v>
+        <v>0.786</v>
       </c>
       <c r="T21" t="n">
-        <v>0.4</v>
+        <v>29861</v>
       </c>
       <c r="U21" t="n">
-        <v>12471</v>
-      </c>
-      <c r="V21" t="n">
-        <v>252</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="V21" t="inlineStr"/>
       <c r="W21" t="inlineStr"/>
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="inlineStr"/>
-      <c r="AB21" t="inlineStr"/>
-      <c r="AC21" t="inlineStr"/>
-      <c r="AD21" t="inlineStr"/>
-      <c r="AE21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>nysd_20_cv_04494</t>
+          <t>nysd_22_cv_10292</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2494,37 +2257,37 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Handelsbanken Fonder AB; Public Employees' Retirement System of Mississippi; State of Rhode Island, Office of the General Treasurer, on behalf of the Employees' Retirement System of Rhode Island; Louisiana Sheriffs' Pension &amp; Relief Fund</t>
+          <t>Steven Christiansen</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Wells Fargo &amp; Company; Timothy J. Sloan; John R. Shrewsberry; Charles W. Scharf; C. Allen Parker; Elizabeth "Betsy" Duke</t>
+          <t>Spectrum Pharmaceuticals, Inc.; Thomas J. Riga; Francois J. Lebel; Nora E. Brennan</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>WFC</t>
+          <t>SPPI</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2018-02-02</t>
+          <t>2022-03-17</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2020-03-12</t>
+          <t>2022-09-22</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and SEC Rule 10b-5</t>
+          <t>Violation of Section 10(b) of the Securities Exchange Act of 1934 and SEC Rule 10b-5</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Exchange Act</t>
+          <t>Violation of Section 20(a) of the Securities Exchange Act of 1934</t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
@@ -2532,43 +2295,36 @@
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="P22" t="n">
-        <v>0.833</v>
+        <v>0.889</v>
       </c>
       <c r="Q22" t="n">
         <v>1</v>
       </c>
       <c r="R22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22" t="n">
-        <v>0.5</v>
+        <v>0.778</v>
       </c>
       <c r="T22" t="n">
-        <v>0.707</v>
+        <v>26601</v>
       </c>
       <c r="U22" t="n">
-        <v>57678</v>
-      </c>
-      <c r="V22" t="n">
-        <v>255</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="V22" t="inlineStr"/>
       <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="inlineStr"/>
-      <c r="AA22" t="inlineStr"/>
-      <c r="AB22" t="inlineStr"/>
-      <c r="AC22" t="inlineStr"/>
-      <c r="AD22" t="inlineStr"/>
-      <c r="AE22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>nysd_22_cv_10292</t>
+          <t>nysd_23_cv_9476</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2581,37 +2337,37 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Steven Christiansen</t>
+          <t>Genesee County Employees' Retirement System</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Spectrum Pharmaceuticals, Inc.; Thomas J. Riga; Francois J. Lebel; Nora E. Brennan</t>
+          <t>DocGo Inc.; Stan Vashovsky; Anthony Capone; Andre Oberholzer</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>SPPI</t>
+          <t>DCGO</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2022-03-17</t>
+          <t>2022-10-11</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2022-09-22</t>
+          <t>2023-09-18</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and Rule 10b-5</t>
+          <t>Violations of Section 10(b) of the Securities Exchange Act of 1934 and SEC Rule 10b-5</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Exchange Act</t>
+          <t>Violations of Section 20(a) of the Securities Exchange Act of 1934</t>
         </is>
       </c>
       <c r="K23" t="inlineStr"/>
@@ -2619,43 +2375,36 @@
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P23" t="n">
-        <v>0.889</v>
+        <v>1</v>
       </c>
       <c r="Q23" t="n">
         <v>1</v>
       </c>
       <c r="R23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S23" t="n">
-        <v>1</v>
+        <v>0.48</v>
       </c>
       <c r="T23" t="n">
-        <v>0.978</v>
+        <v>17444</v>
       </c>
       <c r="U23" t="n">
-        <v>26739</v>
-      </c>
-      <c r="V23" t="n">
-        <v>152</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr"/>
-      <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="inlineStr"/>
-      <c r="AC23" t="inlineStr"/>
-      <c r="AD23" t="inlineStr"/>
-      <c r="AE23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>nysd_23_cv_9476</t>
+          <t>nysd_24_cv_310</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2668,42 +2417,54 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Genesee County Employees' Retirement System</t>
+          <t>The Retirement Plan for Chicago Transit Authority Employees; Oklahoma Firefighters Pension and Retirement System</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>DocGo Inc.; Stan Vashovsky; Anthony Capone; Andre Oberholzer</t>
+          <t>Mobileye Global Inc.; Amnon Shashua; Moran Shemesh Rojansky; Anat Heller; Daniel Galves</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>DCGO</t>
+          <t>MBLY</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2022-04-29</t>
+          <t>2023-01-26</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2023-09-15</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Securities Exchange Act of 1934 and SEC Rule 10b-5</t>
+          <t>Violations of Section 10(b) of the Exchange Act and SEC Rule 10b-5(b)</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Securities Exchange Act of 1934</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
+          <t>Violations of Section 10(b) of the Exchange Act and SEC Rules 10b-5(a) and (c)</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Violations of Section 20(a) of the Exchange Act</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Violations of Section 11 of the Securities Act</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Violations of Section 15 of the Securities Act</t>
+        </is>
+      </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
         <v>0</v>
@@ -2715,34 +2476,27 @@
         <v>1</v>
       </c>
       <c r="R24" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="S24" t="n">
-        <v>0</v>
+        <v>0.72</v>
       </c>
       <c r="T24" t="n">
-        <v>0.5</v>
+        <v>49407</v>
       </c>
       <c r="U24" t="n">
-        <v>17582</v>
-      </c>
-      <c r="V24" t="n">
-        <v>160</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr"/>
-      <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr"/>
-      <c r="AC24" t="inlineStr"/>
-      <c r="AD24" t="inlineStr"/>
-      <c r="AE24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>nysd_24_cv_310</t>
+          <t>txnd-4_24-cv-00673</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2755,93 +2509,74 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>The Retirement Plan for Chicago Transit Authority Employees; Oklahoma Firefighters Pension and Retirement System</t>
+          <t>Dominik Dumancic; Luis Vicente Davidoff Cracasso; Richard Wilkinson</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Mobileye Global Inc.; Amnon Shashua; Moran Shemesh Rojansky; Anat Heller; Daniel Galves</t>
+          <t>American Airlines Group Inc.; Robert D. Isom, Jr.; Devon E. May; Vasu S. Raja</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>MBLY</t>
+          <t>AAL</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2023-01-26</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-05-28</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and SEC Rule 10b-5(b)</t>
+          <t>Violation of Section 10(b) of the Securities Exchange Act of 1934 and Rule 10b-5 promulgated thereunder</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and SEC Rules 10b-5(a) and (c)</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>Section 20(a) of the Exchange Act</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>Section 11 of the Securities Act</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>Section 15 of the Securities Act</t>
-        </is>
-      </c>
+          <t>Violation of Section 20(a) of the Securities Exchange Act of 1934</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
+        <v>1</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>1</v>
+      </c>
+      <c r="R25" t="n">
         <v>0</v>
       </c>
-      <c r="P25" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>1</v>
-      </c>
-      <c r="R25" t="n">
-        <v>1</v>
-      </c>
       <c r="S25" t="n">
-        <v>0.6</v>
+        <v>0.733</v>
       </c>
       <c r="T25" t="n">
-        <v>0.72</v>
+        <v>60140</v>
       </c>
       <c r="U25" t="n">
-        <v>49545</v>
-      </c>
-      <c r="V25" t="n">
-        <v>226</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="V25" t="inlineStr"/>
       <c r="W25" t="inlineStr"/>
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="inlineStr"/>
-      <c r="AA25" t="inlineStr"/>
-      <c r="AB25" t="inlineStr"/>
-      <c r="AC25" t="inlineStr"/>
-      <c r="AD25" t="inlineStr"/>
-      <c r="AE25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>txnd-4_24-cv-00673</t>
+          <t>txsd-4-21-cv-02473</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2854,37 +2589,37 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Dominik Dumancic; Luis Vicente Davidoff Cracasso; Richard Wilkinson</t>
+          <t>Utah Retirement Systems; Construction Laborers Pension Trust for Southern California</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>American Airlines Group Inc.; Robert D. Isom, Jr.; Devon E. May; Vasu S. Raja</t>
+          <t>Concho Resources Inc.; ConocoPhillips; Timothy A. Leach; Jack F. Harper; C. William Giraud; E. Joseph Wright; Brenda R. Schroer</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>AAL</t>
+          <t>CXO</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2023-07-20</t>
+          <t>2018-02-21</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2024-05-28</t>
+          <t>2019-07-31</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Section 10(b) of the Exchange Act and Rule 10b-5</t>
+          <t>Violation of Section 10(b) of the Exchange Act and Rule 10b-5</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Section 20(a) of the Exchange Act</t>
+          <t>Violation of Section 20(a) of the Exchange Act</t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
@@ -2895,7 +2630,7 @@
         <v>1</v>
       </c>
       <c r="P26" t="n">
-        <v>0.667</v>
+        <v>1</v>
       </c>
       <c r="Q26" t="n">
         <v>1</v>
@@ -2907,23 +2642,16 @@
         <v>1</v>
       </c>
       <c r="T26" t="n">
-        <v>0.9330000000000001</v>
+        <v>73892</v>
       </c>
       <c r="U26" t="n">
-        <v>60278</v>
-      </c>
-      <c r="V26" t="n">
-        <v>163</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="V26" t="inlineStr"/>
       <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="inlineStr"/>
-      <c r="AA26" t="inlineStr"/>
-      <c r="AB26" t="inlineStr"/>
-      <c r="AC26" t="inlineStr"/>
-      <c r="AD26" t="inlineStr"/>
-      <c r="AE26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>